<commit_message>
Added Age Match? column to report
</commit_message>
<xml_diff>
--- a/Resources/Geolex_DMU_namescheck.xlsx
+++ b/Resources/Geolex_DMU_namescheck.xlsx
@@ -147,74 +147,6 @@
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -507,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:Q79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
@@ -562,6 +494,7 @@
       <c r="N1" s="7" t="n"/>
       <c r="O1" s="7" t="n"/>
       <c r="P1" s="7" t="n"/>
+      <c r="Q1" s="7" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="8" t="inlineStr">
@@ -636,10 +569,15 @@
       </c>
       <c r="O2" s="11" t="inlineStr">
         <is>
+          <t>Age Match?</t>
+        </is>
+      </c>
+      <c r="P2" s="11" t="inlineStr">
+        <is>
           <t>Remarks</t>
         </is>
       </c>
-      <c r="P2" s="11" t="inlineStr">
+      <c r="Q2" s="11" t="inlineStr">
         <is>
           <t>References</t>
         </is>
@@ -661,7 +599,7 @@
       <c r="E3" s="13" t="inlineStr"/>
       <c r="F3" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G3" s="14" t="inlineStr"/>
@@ -678,6 +616,7 @@
       <c r="N3" s="15" t="inlineStr"/>
       <c r="O3" s="15" t="inlineStr"/>
       <c r="P3" s="15" t="inlineStr"/>
+      <c r="Q3" s="15" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
@@ -707,7 +646,7 @@
       </c>
       <c r="F4" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G4" s="14" t="inlineStr"/>
@@ -724,6 +663,7 @@
       <c r="N4" s="15" t="inlineStr"/>
       <c r="O4" s="15" t="inlineStr"/>
       <c r="P4" s="15" t="inlineStr"/>
+      <c r="Q4" s="15" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="12" t="inlineStr">
@@ -753,7 +693,7 @@
       </c>
       <c r="F5" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G5" s="14" t="inlineStr"/>
@@ -770,6 +710,7 @@
       <c r="N5" s="15" t="inlineStr"/>
       <c r="O5" s="15" t="inlineStr"/>
       <c r="P5" s="15" t="inlineStr"/>
+      <c r="Q5" s="15" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="12" t="inlineStr">
@@ -795,7 +736,7 @@
       </c>
       <c r="F6" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G6" s="14" t="inlineStr"/>
@@ -812,6 +753,7 @@
       <c r="N6" s="15" t="inlineStr"/>
       <c r="O6" s="15" t="inlineStr"/>
       <c r="P6" s="15" t="inlineStr"/>
+      <c r="Q6" s="15" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="12" t="inlineStr">
@@ -837,7 +779,7 @@
       </c>
       <c r="F7" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G7" s="14" t="inlineStr"/>
@@ -854,6 +796,7 @@
       <c r="N7" s="15" t="inlineStr"/>
       <c r="O7" s="15" t="inlineStr"/>
       <c r="P7" s="15" t="inlineStr"/>
+      <c r="Q7" s="15" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="12" t="inlineStr">
@@ -871,7 +814,7 @@
       <c r="E8" s="13" t="inlineStr"/>
       <c r="F8" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G8" s="14" t="inlineStr"/>
@@ -888,6 +831,7 @@
       <c r="N8" s="15" t="inlineStr"/>
       <c r="O8" s="15" t="inlineStr"/>
       <c r="P8" s="15" t="inlineStr"/>
+      <c r="Q8" s="15" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="12" t="inlineStr">
@@ -917,7 +861,7 @@
       </c>
       <c r="F9" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G9" s="14" t="n">
@@ -949,12 +893,13 @@
       </c>
       <c r="M9" s="15" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="N9" s="15" t="inlineStr"/>
       <c r="O9" s="15" t="inlineStr"/>
       <c r="P9" s="15" t="inlineStr"/>
+      <c r="Q9" s="15" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="12" t="inlineStr">
@@ -987,12 +932,13 @@
       <c r="L10" s="14" t="inlineStr"/>
       <c r="M10" s="15" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="N10" s="15" t="inlineStr"/>
       <c r="O10" s="15" t="inlineStr"/>
       <c r="P10" s="15" t="inlineStr"/>
+      <c r="Q10" s="15" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="12" t="inlineStr">
@@ -1022,7 +968,7 @@
       </c>
       <c r="F11" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G11" s="14" t="n">
@@ -1054,12 +1000,13 @@
       </c>
       <c r="M11" s="15" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="N11" s="15" t="inlineStr"/>
       <c r="O11" s="15" t="inlineStr"/>
       <c r="P11" s="15" t="inlineStr"/>
+      <c r="Q11" s="15" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
@@ -1092,12 +1039,13 @@
       <c r="L12" s="14" t="inlineStr"/>
       <c r="M12" s="15" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="N12" s="15" t="inlineStr"/>
       <c r="O12" s="15" t="inlineStr"/>
       <c r="P12" s="15" t="inlineStr"/>
+      <c r="Q12" s="15" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="12" t="inlineStr">
@@ -1130,12 +1078,13 @@
       <c r="L13" s="14" t="inlineStr"/>
       <c r="M13" s="15" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="N13" s="15" t="inlineStr"/>
       <c r="O13" s="15" t="inlineStr"/>
       <c r="P13" s="15" t="inlineStr"/>
+      <c r="Q13" s="15" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="12" t="inlineStr">
@@ -1174,6 +1123,7 @@
       <c r="N14" s="15" t="inlineStr"/>
       <c r="O14" s="15" t="inlineStr"/>
       <c r="P14" s="15" t="inlineStr"/>
+      <c r="Q14" s="15" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
@@ -1212,6 +1162,7 @@
       <c r="N15" s="15" t="inlineStr"/>
       <c r="O15" s="15" t="inlineStr"/>
       <c r="P15" s="15" t="inlineStr"/>
+      <c r="Q15" s="15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="12" t="inlineStr">
@@ -1250,6 +1201,7 @@
       <c r="N16" s="15" t="inlineStr"/>
       <c r="O16" s="15" t="inlineStr"/>
       <c r="P16" s="15" t="inlineStr"/>
+      <c r="Q16" s="15" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="12" t="inlineStr">
@@ -1291,12 +1243,13 @@
       </c>
       <c r="M17" s="15" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="N17" s="15" t="inlineStr"/>
       <c r="O17" s="15" t="inlineStr"/>
       <c r="P17" s="15" t="inlineStr"/>
+      <c r="Q17" s="15" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="12" t="inlineStr">
@@ -1329,12 +1282,13 @@
       <c r="L18" s="14" t="inlineStr"/>
       <c r="M18" s="15" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="N18" s="15" t="inlineStr"/>
       <c r="O18" s="15" t="inlineStr"/>
       <c r="P18" s="15" t="inlineStr"/>
+      <c r="Q18" s="15" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="12" t="inlineStr">
@@ -1373,6 +1327,7 @@
       <c r="N19" s="15" t="inlineStr"/>
       <c r="O19" s="15" t="inlineStr"/>
       <c r="P19" s="15" t="inlineStr"/>
+      <c r="Q19" s="15" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="12" t="inlineStr">
@@ -1402,7 +1357,7 @@
       </c>
       <c r="F20" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G20" s="14" t="n">
@@ -1436,6 +1391,7 @@
       <c r="N20" s="15" t="inlineStr"/>
       <c r="O20" s="15" t="inlineStr"/>
       <c r="P20" s="15" t="inlineStr"/>
+      <c r="Q20" s="15" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="12" t="inlineStr">
@@ -1465,7 +1421,7 @@
       </c>
       <c r="F21" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G21" s="14" t="n">
@@ -1503,6 +1459,7 @@
       <c r="N21" s="15" t="inlineStr"/>
       <c r="O21" s="15" t="inlineStr"/>
       <c r="P21" s="15" t="inlineStr"/>
+      <c r="Q21" s="15" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="12" t="inlineStr">
@@ -1532,7 +1489,7 @@
       </c>
       <c r="F22" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G22" s="14" t="n">
@@ -1570,6 +1527,7 @@
       <c r="N22" s="15" t="inlineStr"/>
       <c r="O22" s="15" t="inlineStr"/>
       <c r="P22" s="15" t="inlineStr"/>
+      <c r="Q22" s="15" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="12" t="inlineStr">
@@ -1617,6 +1575,7 @@
       <c r="N23" s="15" t="inlineStr"/>
       <c r="O23" s="15" t="inlineStr"/>
       <c r="P23" s="15" t="inlineStr"/>
+      <c r="Q23" s="15" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="12" t="inlineStr">
@@ -1655,6 +1614,7 @@
       <c r="N24" s="15" t="inlineStr"/>
       <c r="O24" s="15" t="inlineStr"/>
       <c r="P24" s="15" t="inlineStr"/>
+      <c r="Q24" s="15" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="12" t="inlineStr">
@@ -1702,6 +1662,7 @@
       <c r="N25" s="15" t="inlineStr"/>
       <c r="O25" s="15" t="inlineStr"/>
       <c r="P25" s="15" t="inlineStr"/>
+      <c r="Q25" s="15" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="12" t="inlineStr">
@@ -1740,6 +1701,7 @@
       <c r="N26" s="15" t="inlineStr"/>
       <c r="O26" s="15" t="inlineStr"/>
       <c r="P26" s="15" t="inlineStr"/>
+      <c r="Q26" s="15" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="12" t="inlineStr">
@@ -1769,7 +1731,7 @@
       </c>
       <c r="F27" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G27" s="14" t="n">
@@ -1807,6 +1769,7 @@
       <c r="N27" s="15" t="inlineStr"/>
       <c r="O27" s="15" t="inlineStr"/>
       <c r="P27" s="15" t="inlineStr"/>
+      <c r="Q27" s="15" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="12" t="inlineStr">
@@ -1845,6 +1808,7 @@
       <c r="N28" s="15" t="inlineStr"/>
       <c r="O28" s="15" t="inlineStr"/>
       <c r="P28" s="15" t="inlineStr"/>
+      <c r="Q28" s="15" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="12" t="inlineStr">
@@ -1879,6 +1843,7 @@
       <c r="N29" s="15" t="inlineStr"/>
       <c r="O29" s="15" t="inlineStr"/>
       <c r="P29" s="15" t="inlineStr"/>
+      <c r="Q29" s="15" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="12" t="inlineStr">
@@ -1926,6 +1891,7 @@
       <c r="N30" s="15" t="inlineStr"/>
       <c r="O30" s="15" t="inlineStr"/>
       <c r="P30" s="15" t="inlineStr"/>
+      <c r="Q30" s="15" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="12" t="inlineStr">
@@ -1964,6 +1930,7 @@
       <c r="N31" s="15" t="inlineStr"/>
       <c r="O31" s="15" t="inlineStr"/>
       <c r="P31" s="15" t="inlineStr"/>
+      <c r="Q31" s="15" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="12" t="inlineStr">
@@ -1993,7 +1960,7 @@
       </c>
       <c r="F32" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G32" s="14" t="n">
@@ -2031,6 +1998,7 @@
       <c r="N32" s="15" t="inlineStr"/>
       <c r="O32" s="15" t="inlineStr"/>
       <c r="P32" s="15" t="inlineStr"/>
+      <c r="Q32" s="15" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="12" t="inlineStr">
@@ -2048,7 +2016,7 @@
       <c r="E33" s="13" t="inlineStr"/>
       <c r="F33" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G33" s="14" t="inlineStr"/>
@@ -2065,6 +2033,7 @@
       <c r="N33" s="15" t="inlineStr"/>
       <c r="O33" s="15" t="inlineStr"/>
       <c r="P33" s="15" t="inlineStr"/>
+      <c r="Q33" s="15" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="12" t="inlineStr">
@@ -2090,7 +2059,7 @@
       </c>
       <c r="F34" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G34" s="14" t="n">
@@ -2128,6 +2097,7 @@
       <c r="N34" s="15" t="inlineStr"/>
       <c r="O34" s="15" t="inlineStr"/>
       <c r="P34" s="15" t="inlineStr"/>
+      <c r="Q34" s="15" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="12" t="inlineStr">
@@ -2160,12 +2130,13 @@
       <c r="L35" s="14" t="inlineStr"/>
       <c r="M35" s="15" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="N35" s="15" t="inlineStr"/>
       <c r="O35" s="15" t="inlineStr"/>
       <c r="P35" s="15" t="inlineStr"/>
+      <c r="Q35" s="15" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="12" t="inlineStr">
@@ -2198,12 +2169,13 @@
       <c r="L36" s="14" t="inlineStr"/>
       <c r="M36" s="15" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="N36" s="15" t="inlineStr"/>
       <c r="O36" s="15" t="inlineStr"/>
       <c r="P36" s="15" t="inlineStr"/>
+      <c r="Q36" s="15" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="12" t="inlineStr">
@@ -2242,6 +2214,7 @@
       <c r="N37" s="15" t="inlineStr"/>
       <c r="O37" s="15" t="inlineStr"/>
       <c r="P37" s="15" t="inlineStr"/>
+      <c r="Q37" s="15" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="12" t="inlineStr">
@@ -2289,6 +2262,7 @@
       <c r="N38" s="15" t="inlineStr"/>
       <c r="O38" s="15" t="inlineStr"/>
       <c r="P38" s="15" t="inlineStr"/>
+      <c r="Q38" s="15" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="12" t="inlineStr">
@@ -2327,6 +2301,7 @@
       <c r="N39" s="15" t="inlineStr"/>
       <c r="O39" s="15" t="inlineStr"/>
       <c r="P39" s="15" t="inlineStr"/>
+      <c r="Q39" s="15" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="12" t="inlineStr">
@@ -2365,6 +2340,7 @@
       <c r="N40" s="15" t="inlineStr"/>
       <c r="O40" s="15" t="inlineStr"/>
       <c r="P40" s="15" t="inlineStr"/>
+      <c r="Q40" s="15" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="12" t="inlineStr">
@@ -2412,6 +2388,7 @@
       <c r="N41" s="15" t="inlineStr"/>
       <c r="O41" s="15" t="inlineStr"/>
       <c r="P41" s="15" t="inlineStr"/>
+      <c r="Q41" s="15" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="12" t="inlineStr">
@@ -2459,6 +2436,7 @@
       <c r="N42" s="15" t="inlineStr"/>
       <c r="O42" s="15" t="inlineStr"/>
       <c r="P42" s="15" t="inlineStr"/>
+      <c r="Q42" s="15" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="12" t="inlineStr">
@@ -2484,7 +2462,7 @@
       </c>
       <c r="F43" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G43" s="14" t="n">
@@ -2522,6 +2500,7 @@
       <c r="N43" s="15" t="inlineStr"/>
       <c r="O43" s="15" t="inlineStr"/>
       <c r="P43" s="15" t="inlineStr"/>
+      <c r="Q43" s="15" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="12" t="inlineStr">
@@ -2547,7 +2526,7 @@
       </c>
       <c r="F44" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G44" s="14" t="n">
@@ -2585,6 +2564,7 @@
       <c r="N44" s="15" t="inlineStr"/>
       <c r="O44" s="15" t="inlineStr"/>
       <c r="P44" s="15" t="inlineStr"/>
+      <c r="Q44" s="15" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="12" t="inlineStr">
@@ -2632,6 +2612,7 @@
       <c r="N45" s="15" t="inlineStr"/>
       <c r="O45" s="15" t="inlineStr"/>
       <c r="P45" s="15" t="inlineStr"/>
+      <c r="Q45" s="15" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="12" t="inlineStr">
@@ -2649,7 +2630,7 @@
       <c r="E46" s="13" t="inlineStr"/>
       <c r="F46" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G46" s="14" t="n">
@@ -2687,6 +2668,7 @@
       <c r="N46" s="15" t="inlineStr"/>
       <c r="O46" s="15" t="inlineStr"/>
       <c r="P46" s="15" t="inlineStr"/>
+      <c r="Q46" s="15" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="12" t="inlineStr">
@@ -2725,6 +2707,7 @@
       <c r="N47" s="15" t="inlineStr"/>
       <c r="O47" s="15" t="inlineStr"/>
       <c r="P47" s="15" t="inlineStr"/>
+      <c r="Q47" s="15" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="12" t="inlineStr">
@@ -2742,7 +2725,7 @@
       <c r="E48" s="13" t="inlineStr"/>
       <c r="F48" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G48" s="14" t="inlineStr"/>
@@ -2759,6 +2742,7 @@
       <c r="N48" s="15" t="inlineStr"/>
       <c r="O48" s="15" t="inlineStr"/>
       <c r="P48" s="15" t="inlineStr"/>
+      <c r="Q48" s="15" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="12" t="inlineStr">
@@ -2788,7 +2772,7 @@
       </c>
       <c r="F49" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G49" s="14" t="n">
@@ -2826,6 +2810,7 @@
       <c r="N49" s="15" t="inlineStr"/>
       <c r="O49" s="15" t="inlineStr"/>
       <c r="P49" s="15" t="inlineStr"/>
+      <c r="Q49" s="15" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="12" t="inlineStr">
@@ -2855,7 +2840,7 @@
       </c>
       <c r="F50" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G50" s="14" t="n">
@@ -2893,6 +2878,7 @@
       <c r="N50" s="15" t="inlineStr"/>
       <c r="O50" s="15" t="inlineStr"/>
       <c r="P50" s="15" t="inlineStr"/>
+      <c r="Q50" s="15" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="12" t="inlineStr">
@@ -2931,6 +2917,7 @@
       <c r="N51" s="15" t="inlineStr"/>
       <c r="O51" s="15" t="inlineStr"/>
       <c r="P51" s="15" t="inlineStr"/>
+      <c r="Q51" s="15" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="12" t="inlineStr">
@@ -2960,7 +2947,7 @@
       </c>
       <c r="F52" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G52" s="14" t="n">
@@ -2998,6 +2985,7 @@
       <c r="N52" s="15" t="inlineStr"/>
       <c r="O52" s="15" t="inlineStr"/>
       <c r="P52" s="15" t="inlineStr"/>
+      <c r="Q52" s="15" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="12" t="inlineStr">
@@ -3027,7 +3015,7 @@
       </c>
       <c r="F53" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G53" s="14" t="n">
@@ -3065,6 +3053,7 @@
       <c r="N53" s="15" t="inlineStr"/>
       <c r="O53" s="15" t="inlineStr"/>
       <c r="P53" s="15" t="inlineStr"/>
+      <c r="Q53" s="15" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="12" t="inlineStr">
@@ -3087,12 +3076,14 @@
           <t>Lewis Shale</t>
         </is>
       </c>
-      <c r="E54" s="13" t="n">
-        <v>15</v>
+      <c r="E54" s="13" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
       <c r="F54" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G54" s="14" t="n">
@@ -3130,6 +3121,7 @@
       <c r="N54" s="15" t="inlineStr"/>
       <c r="O54" s="15" t="inlineStr"/>
       <c r="P54" s="15" t="inlineStr"/>
+      <c r="Q54" s="15" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="12" t="inlineStr">
@@ -3168,6 +3160,7 @@
       <c r="N55" s="15" t="inlineStr"/>
       <c r="O55" s="15" t="inlineStr"/>
       <c r="P55" s="15" t="inlineStr"/>
+      <c r="Q55" s="15" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="12" t="inlineStr">
@@ -3215,6 +3208,7 @@
       <c r="N56" s="15" t="inlineStr"/>
       <c r="O56" s="15" t="inlineStr"/>
       <c r="P56" s="15" t="inlineStr"/>
+      <c r="Q56" s="15" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="12" t="inlineStr">
@@ -3244,7 +3238,7 @@
       </c>
       <c r="F57" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G57" s="14" t="n">
@@ -3282,6 +3276,7 @@
       <c r="N57" s="15" t="inlineStr"/>
       <c r="O57" s="15" t="inlineStr"/>
       <c r="P57" s="15" t="inlineStr"/>
+      <c r="Q57" s="15" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="12" t="inlineStr">
@@ -3311,7 +3306,7 @@
       </c>
       <c r="F58" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G58" s="14" t="n">
@@ -3349,6 +3344,7 @@
       <c r="N58" s="15" t="inlineStr"/>
       <c r="O58" s="15" t="inlineStr"/>
       <c r="P58" s="15" t="inlineStr"/>
+      <c r="Q58" s="15" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="12" t="inlineStr">
@@ -3387,6 +3383,7 @@
       <c r="N59" s="15" t="inlineStr"/>
       <c r="O59" s="15" t="inlineStr"/>
       <c r="P59" s="15" t="inlineStr"/>
+      <c r="Q59" s="15" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="12" t="inlineStr">
@@ -3425,6 +3422,7 @@
       <c r="N60" s="15" t="inlineStr"/>
       <c r="O60" s="15" t="inlineStr"/>
       <c r="P60" s="15" t="inlineStr"/>
+      <c r="Q60" s="15" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="12" t="inlineStr">
@@ -3463,6 +3461,7 @@
       <c r="N61" s="15" t="inlineStr"/>
       <c r="O61" s="15" t="inlineStr"/>
       <c r="P61" s="15" t="inlineStr"/>
+      <c r="Q61" s="15" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="12" t="inlineStr">
@@ -3492,7 +3491,7 @@
       </c>
       <c r="F62" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G62" s="14" t="n">
@@ -3530,6 +3529,7 @@
       <c r="N62" s="15" t="inlineStr"/>
       <c r="O62" s="15" t="inlineStr"/>
       <c r="P62" s="15" t="inlineStr"/>
+      <c r="Q62" s="15" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="12" t="inlineStr">
@@ -3547,7 +3547,7 @@
       <c r="E63" s="13" t="inlineStr"/>
       <c r="F63" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G63" s="14" t="inlineStr"/>
@@ -3564,6 +3564,7 @@
       <c r="N63" s="15" t="inlineStr"/>
       <c r="O63" s="15" t="inlineStr"/>
       <c r="P63" s="15" t="inlineStr"/>
+      <c r="Q63" s="15" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="12" t="inlineStr">
@@ -3593,7 +3594,7 @@
       </c>
       <c r="F64" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G64" s="14" t="n">
@@ -3631,6 +3632,7 @@
       <c r="N64" s="15" t="inlineStr"/>
       <c r="O64" s="15" t="inlineStr"/>
       <c r="P64" s="15" t="inlineStr"/>
+      <c r="Q64" s="15" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="12" t="inlineStr">
@@ -3669,6 +3671,7 @@
       <c r="N65" s="15" t="inlineStr"/>
       <c r="O65" s="15" t="inlineStr"/>
       <c r="P65" s="15" t="inlineStr"/>
+      <c r="Q65" s="15" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="12" t="inlineStr">
@@ -3716,6 +3719,7 @@
       <c r="N66" s="15" t="inlineStr"/>
       <c r="O66" s="15" t="inlineStr"/>
       <c r="P66" s="15" t="inlineStr"/>
+      <c r="Q66" s="15" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="12" t="inlineStr">
@@ -3763,6 +3767,7 @@
       <c r="N67" s="15" t="inlineStr"/>
       <c r="O67" s="15" t="inlineStr"/>
       <c r="P67" s="15" t="inlineStr"/>
+      <c r="Q67" s="15" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="12" t="inlineStr">
@@ -3788,7 +3793,7 @@
       <c r="E68" s="13" t="inlineStr"/>
       <c r="F68" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G68" s="14" t="inlineStr"/>
@@ -3805,6 +3810,7 @@
       <c r="N68" s="15" t="inlineStr"/>
       <c r="O68" s="15" t="inlineStr"/>
       <c r="P68" s="15" t="inlineStr"/>
+      <c r="Q68" s="15" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="12" t="inlineStr">
@@ -3834,7 +3840,7 @@
       </c>
       <c r="F69" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G69" s="14" t="n">
@@ -3872,6 +3878,7 @@
       <c r="N69" s="15" t="inlineStr"/>
       <c r="O69" s="15" t="inlineStr"/>
       <c r="P69" s="15" t="inlineStr"/>
+      <c r="Q69" s="15" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="12" t="inlineStr">
@@ -3901,7 +3908,7 @@
       </c>
       <c r="F70" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G70" s="14" t="n">
@@ -3939,6 +3946,7 @@
       <c r="N70" s="15" t="inlineStr"/>
       <c r="O70" s="15" t="inlineStr"/>
       <c r="P70" s="15" t="inlineStr"/>
+      <c r="Q70" s="15" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="12" t="inlineStr">
@@ -3956,7 +3964,7 @@
       <c r="E71" s="13" t="inlineStr"/>
       <c r="F71" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G71" s="14" t="inlineStr"/>
@@ -3973,6 +3981,7 @@
       <c r="N71" s="15" t="inlineStr"/>
       <c r="O71" s="15" t="inlineStr"/>
       <c r="P71" s="15" t="inlineStr"/>
+      <c r="Q71" s="15" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="12" t="inlineStr">
@@ -4002,7 +4011,7 @@
       </c>
       <c r="F72" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G72" s="14" t="n">
@@ -4040,6 +4049,7 @@
       <c r="N72" s="15" t="inlineStr"/>
       <c r="O72" s="15" t="inlineStr"/>
       <c r="P72" s="15" t="inlineStr"/>
+      <c r="Q72" s="15" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="12" t="inlineStr">
@@ -4078,6 +4088,7 @@
       <c r="N73" s="15" t="inlineStr"/>
       <c r="O73" s="15" t="inlineStr"/>
       <c r="P73" s="15" t="inlineStr"/>
+      <c r="Q73" s="15" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="12" t="inlineStr">
@@ -4107,7 +4118,7 @@
       </c>
       <c r="F74" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G74" s="14" t="n">
@@ -4145,6 +4156,7 @@
       <c r="N74" s="15" t="inlineStr"/>
       <c r="O74" s="15" t="inlineStr"/>
       <c r="P74" s="15" t="inlineStr"/>
+      <c r="Q74" s="15" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="12" t="inlineStr">
@@ -4183,6 +4195,7 @@
       <c r="N75" s="15" t="inlineStr"/>
       <c r="O75" s="15" t="inlineStr"/>
       <c r="P75" s="15" t="inlineStr"/>
+      <c r="Q75" s="15" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="12" t="inlineStr">
@@ -4212,7 +4225,7 @@
       </c>
       <c r="F76" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">oh, </t>
+          <t>OH, PA, WV, VA</t>
         </is>
       </c>
       <c r="G76" s="14" t="n">
@@ -4250,6 +4263,7 @@
       <c r="N76" s="15" t="inlineStr"/>
       <c r="O76" s="15" t="inlineStr"/>
       <c r="P76" s="15" t="inlineStr"/>
+      <c r="Q76" s="15" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="12" t="inlineStr">
@@ -4288,6 +4302,7 @@
       <c r="N77" s="15" t="inlineStr"/>
       <c r="O77" s="15" t="inlineStr"/>
       <c r="P77" s="15" t="inlineStr"/>
+      <c r="Q77" s="15" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="12" t="inlineStr">
@@ -4335,6 +4350,7 @@
       <c r="N78" s="15" t="inlineStr"/>
       <c r="O78" s="15" t="inlineStr"/>
       <c r="P78" s="15" t="inlineStr"/>
+      <c r="Q78" s="15" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="12" t="inlineStr">
@@ -4373,12 +4389,13 @@
       <c r="N79" s="15" t="inlineStr"/>
       <c r="O79" s="15" t="inlineStr"/>
       <c r="P79" s="15" t="inlineStr"/>
+      <c r="Q79" s="15" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:L1"/>
-    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="M1:Q1"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
unimportant change to demo output from names check tool
</commit_message>
<xml_diff>
--- a/Resources/Geolex_DMU_namescheck.xlsx
+++ b/Resources/Geolex_DMU_namescheck.xlsx
@@ -669,7 +669,7 @@
       <c r="E3" s="13" t="inlineStr"/>
       <c r="F3" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G3" s="14" t="inlineStr"/>
@@ -716,7 +716,7 @@
       </c>
       <c r="F4" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G4" s="14" t="inlineStr"/>
@@ -763,7 +763,7 @@
       </c>
       <c r="F5" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G5" s="14" t="inlineStr"/>
@@ -806,7 +806,7 @@
       </c>
       <c r="F6" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G6" s="14" t="inlineStr"/>
@@ -849,7 +849,7 @@
       </c>
       <c r="F7" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G7" s="14" t="inlineStr"/>
@@ -884,7 +884,7 @@
       <c r="E8" s="13" t="inlineStr"/>
       <c r="F8" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G8" s="14" t="inlineStr"/>
@@ -931,7 +931,7 @@
       </c>
       <c r="F9" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G9" s="14" t="n">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="F11" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G11" s="14" t="n">
@@ -1148,7 +1148,7 @@
       <c r="L13" s="14" t="inlineStr"/>
       <c r="M13" s="15" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="N13" s="15" t="inlineStr"/>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="F20" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G20" s="14" t="n">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="F21" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G21" s="14" t="n">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="F22" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G22" s="14" t="n">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="F27" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G27" s="14" t="n">
@@ -2030,7 +2030,7 @@
       </c>
       <c r="F32" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G32" s="14" t="n">
@@ -2086,7 +2086,7 @@
       <c r="E33" s="13" t="inlineStr"/>
       <c r="F33" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G33" s="14" t="inlineStr"/>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="F34" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G34" s="14" t="n">
@@ -2239,7 +2239,7 @@
       <c r="L36" s="14" t="inlineStr"/>
       <c r="M36" s="15" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="N36" s="15" t="inlineStr"/>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="F43" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G43" s="14" t="n">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="F44" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G44" s="14" t="n">
@@ -2700,7 +2700,7 @@
       <c r="E46" s="13" t="inlineStr"/>
       <c r="F46" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G46" s="14" t="n">
@@ -2795,7 +2795,7 @@
       <c r="E48" s="13" t="inlineStr"/>
       <c r="F48" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G48" s="14" t="inlineStr"/>
@@ -2842,7 +2842,7 @@
       </c>
       <c r="F49" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G49" s="14" t="n">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="F50" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G50" s="14" t="n">
@@ -3017,7 +3017,7 @@
       </c>
       <c r="F52" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G52" s="14" t="n">
@@ -3085,7 +3085,7 @@
       </c>
       <c r="F53" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G53" s="14" t="n">
@@ -3153,7 +3153,7 @@
       </c>
       <c r="F54" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G54" s="14" t="n">
@@ -3308,7 +3308,7 @@
       </c>
       <c r="F57" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G57" s="14" t="n">
@@ -3376,7 +3376,7 @@
       </c>
       <c r="F58" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G58" s="14" t="n">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="F62" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G62" s="14" t="n">
@@ -3617,7 +3617,7 @@
       <c r="E63" s="13" t="inlineStr"/>
       <c r="F63" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G63" s="14" t="inlineStr"/>
@@ -3664,7 +3664,7 @@
       </c>
       <c r="F64" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G64" s="14" t="n">
@@ -3863,7 +3863,7 @@
       <c r="E68" s="13" t="inlineStr"/>
       <c r="F68" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G68" s="14" t="inlineStr"/>
@@ -3910,7 +3910,7 @@
       </c>
       <c r="F69" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G69" s="14" t="n">
@@ -3978,7 +3978,7 @@
       </c>
       <c r="F70" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G70" s="14" t="n">
@@ -4034,7 +4034,7 @@
       <c r="E71" s="13" t="inlineStr"/>
       <c r="F71" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G71" s="14" t="inlineStr"/>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="F72" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G72" s="14" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="F74" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G74" s="14" t="n">
@@ -4295,7 +4295,7 @@
       </c>
       <c r="F76" s="13" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>WV, VA</t>
         </is>
       </c>
       <c r="G76" s="14" t="n">

</xml_diff>

<commit_message>
added readme for name check tool
</commit_message>
<xml_diff>
--- a/Resources/Geolex_DMU_namescheck.xlsx
+++ b/Resources/Geolex_DMU_namescheck.xlsx
@@ -669,7 +669,7 @@
       <c r="E3" s="13" t="inlineStr"/>
       <c r="F3" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G3" s="14" t="inlineStr"/>
@@ -716,7 +716,7 @@
       </c>
       <c r="F4" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G4" s="14" t="inlineStr"/>
@@ -763,7 +763,7 @@
       </c>
       <c r="F5" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G5" s="14" t="inlineStr"/>
@@ -806,7 +806,7 @@
       </c>
       <c r="F6" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G6" s="14" t="inlineStr"/>
@@ -849,7 +849,7 @@
       </c>
       <c r="F7" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G7" s="14" t="inlineStr"/>
@@ -884,7 +884,7 @@
       <c r="E8" s="13" t="inlineStr"/>
       <c r="F8" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G8" s="14" t="inlineStr"/>
@@ -931,7 +931,7 @@
       </c>
       <c r="F9" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G9" s="14" t="n">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="F11" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G11" s="14" t="n">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="F20" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G20" s="14" t="n">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="F21" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G21" s="14" t="n">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="F22" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G22" s="14" t="n">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="F27" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G27" s="14" t="n">
@@ -2030,7 +2030,7 @@
       </c>
       <c r="F32" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G32" s="14" t="n">
@@ -2086,7 +2086,7 @@
       <c r="E33" s="13" t="inlineStr"/>
       <c r="F33" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G33" s="14" t="inlineStr"/>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="F34" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G34" s="14" t="n">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="F43" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G43" s="14" t="n">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="F44" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G44" s="14" t="n">
@@ -2700,7 +2700,7 @@
       <c r="E46" s="13" t="inlineStr"/>
       <c r="F46" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G46" s="14" t="n">
@@ -2795,7 +2795,7 @@
       <c r="E48" s="13" t="inlineStr"/>
       <c r="F48" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G48" s="14" t="inlineStr"/>
@@ -2842,7 +2842,7 @@
       </c>
       <c r="F49" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G49" s="14" t="n">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="F50" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G50" s="14" t="n">
@@ -3017,7 +3017,7 @@
       </c>
       <c r="F52" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G52" s="14" t="n">
@@ -3085,7 +3085,7 @@
       </c>
       <c r="F53" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G53" s="14" t="n">
@@ -3153,7 +3153,7 @@
       </c>
       <c r="F54" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G54" s="14" t="n">
@@ -3308,7 +3308,7 @@
       </c>
       <c r="F57" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G57" s="14" t="n">
@@ -3376,7 +3376,7 @@
       </c>
       <c r="F58" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G58" s="14" t="n">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="F62" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G62" s="14" t="n">
@@ -3617,7 +3617,7 @@
       <c r="E63" s="13" t="inlineStr"/>
       <c r="F63" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G63" s="14" t="inlineStr"/>
@@ -3664,7 +3664,7 @@
       </c>
       <c r="F64" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G64" s="14" t="n">
@@ -3863,7 +3863,7 @@
       <c r="E68" s="13" t="inlineStr"/>
       <c r="F68" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G68" s="14" t="inlineStr"/>
@@ -3910,7 +3910,7 @@
       </c>
       <c r="F69" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G69" s="14" t="n">
@@ -3978,7 +3978,7 @@
       </c>
       <c r="F70" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G70" s="14" t="n">
@@ -4034,7 +4034,7 @@
       <c r="E71" s="13" t="inlineStr"/>
       <c r="F71" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G71" s="14" t="inlineStr"/>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="F72" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G72" s="14" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="F74" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G74" s="14" t="n">
@@ -4295,7 +4295,7 @@
       </c>
       <c r="F76" s="13" t="inlineStr">
         <is>
-          <t>WV, VA</t>
+          <t>VA, WV</t>
         </is>
       </c>
       <c r="G76" s="14" t="n">

</xml_diff>